<commit_message>
Seguimos actualizando paquetes a español apertura
</commit_message>
<xml_diff>
--- a/APP_PERSONAS_XML/src/test/resources/datadriven/inversionvirtual/Trn_0326Apertura.xlsx
+++ b/APP_PERSONAS_XML/src/test/resources/datadriven/inversionvirtual/Trn_0326Apertura.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATIZACION JAVA\PROYECTOS GRADLE\PROYECTOS XML\PITTS_CanalesVirtuales_XML_TEST\src\test\resources\datadriven\virtualinvestment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATIZACION JAVA\PROYECTOS GRADLE\PROYECTOS NUEVA APP\AW1059001_NuevaAPPSucursalVirtualPersonas_Test\APP_PERSONAS_XML\src\test\resources\datadriven\inversionvirtual\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -183,16 +183,16 @@
     <t>40676340007</t>
   </si>
   <si>
-    <t>5150000</t>
-  </si>
-  <si>
-    <t>5160000</t>
-  </si>
-  <si>
     <t>2443</t>
   </si>
   <si>
     <t>4321</t>
+  </si>
+  <si>
+    <t>516000</t>
+  </si>
+  <si>
+    <t>550000</t>
   </si>
 </sst>
 </file>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -692,10 +692,10 @@
         <v>49</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>4</v>
@@ -716,7 +716,7 @@
         <v>30</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>46</v>
@@ -745,10 +745,10 @@
         <v>49</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>4</v>
@@ -769,7 +769,7 @@
         <v>30</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Actualizacion datadriven y feature apertura
</commit_message>
<xml_diff>
--- a/APP_PERSONAS_XML/src/test/resources/datadriven/inversionvirtual/Trn_0326Apertura.xlsx
+++ b/APP_PERSONAS_XML/src/test/resources/datadriven/inversionvirtual/Trn_0326Apertura.xlsx
@@ -189,10 +189,10 @@
     <t>4321</t>
   </si>
   <si>
-    <t>516000</t>
-  </si>
-  <si>
     <t>550000</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -716,7 +716,7 @@
         <v>30</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>46</v>
@@ -751,7 +751,7 @@
         <v>52</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>5</v>
@@ -769,7 +769,7 @@
         <v>30</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>45</v>

</xml_diff>